<commit_message>
Merged NTE and NTW into NTN (4 areas in total)
</commit_message>
<xml_diff>
--- a/dat/cases/hk_annual_cases_areas.xlsx
+++ b/dat/cases/hk_annual_cases_areas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>year</t>
   </si>
@@ -42,6 +42,9 @@
   </si>
   <si>
     <t>NTW</t>
+  </si>
+  <si>
+    <t>NTN</t>
   </si>
 </sst>
 </file>
@@ -359,15 +362,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:G18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J23" sqref="J23"/>
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,8 +389,11 @@
       <c r="F1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -406,8 +412,11 @@
       <c r="F2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G2">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -426,8 +435,11 @@
       <c r="F3">
         <v>0</v>
       </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2004</v>
       </c>
@@ -446,8 +458,11 @@
       <c r="F4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2005</v>
       </c>
@@ -466,8 +481,11 @@
       <c r="F5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -486,8 +504,11 @@
       <c r="F6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -506,8 +527,11 @@
       <c r="F7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -526,8 +550,11 @@
       <c r="F8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -546,8 +573,11 @@
       <c r="F9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -566,8 +596,11 @@
       <c r="F10">
         <v>4</v>
       </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -586,8 +619,11 @@
       <c r="F11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -606,8 +642,11 @@
       <c r="F12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -626,8 +665,11 @@
       <c r="F13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -646,8 +688,11 @@
       <c r="F14">
         <v>2</v>
       </c>
-    </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -666,8 +711,11 @@
       <c r="F15">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -686,8 +734,11 @@
       <c r="F16">
         <v>3</v>
       </c>
-    </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G16">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -706,8 +757,11 @@
       <c r="F17">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2018</v>
       </c>
@@ -724,6 +778,9 @@
         <v>18</v>
       </c>
       <c r="F18">
+        <v>0</v>
+      </c>
+      <c r="G18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Wrote custom step aic (stepAIC_custom.R) for general models
</commit_message>
<xml_diff>
--- a/dat/cases/hk_annual_cases_areas.xlsx
+++ b/dat/cases/hk_annual_cases_areas.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>year</t>
   </si>
@@ -35,13 +35,7 @@
     <t>NTS</t>
   </si>
   <si>
-    <t>NTE</t>
-  </si>
-  <si>
     <t>KL</t>
-  </si>
-  <si>
-    <t>NTW</t>
   </si>
   <si>
     <t>NTN</t>
@@ -362,15 +356,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G18"/>
+  <dimension ref="A1:E18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -381,19 +375,13 @@
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -401,22 +389,16 @@
         <v>0</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
+        <v>0</v>
+      </c>
+      <c r="E2">
         <v>20</v>
       </c>
-      <c r="D2">
-        <v>0</v>
-      </c>
-      <c r="E2">
-        <v>0</v>
-      </c>
-      <c r="F2">
-        <v>0</v>
-      </c>
-      <c r="G2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -427,19 +409,13 @@
         <v>0</v>
       </c>
       <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="E3">
         <v>1</v>
       </c>
-      <c r="E3">
-        <v>0</v>
-      </c>
-      <c r="F3">
-        <v>0</v>
-      </c>
-      <c r="G3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2004</v>
       </c>
@@ -455,14 +431,8 @@
       <c r="E4">
         <v>0</v>
       </c>
-      <c r="F4">
-        <v>0</v>
-      </c>
-      <c r="G4">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2005</v>
       </c>
@@ -478,14 +448,8 @@
       <c r="E5">
         <v>0</v>
       </c>
-      <c r="F5">
-        <v>0</v>
-      </c>
-      <c r="G5">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -501,14 +465,8 @@
       <c r="E6">
         <v>0</v>
       </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -524,14 +482,8 @@
       <c r="E7">
         <v>0</v>
       </c>
-      <c r="F7">
-        <v>0</v>
-      </c>
-      <c r="G7">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -547,14 +499,8 @@
       <c r="E8">
         <v>0</v>
       </c>
-      <c r="F8">
-        <v>0</v>
-      </c>
-      <c r="G8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -570,14 +516,8 @@
       <c r="E9">
         <v>0</v>
       </c>
-      <c r="F9">
-        <v>0</v>
-      </c>
-      <c r="G9">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -588,19 +528,13 @@
         <v>0</v>
       </c>
       <c r="D10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="E10">
         <v>0</v>
       </c>
-      <c r="F10">
-        <v>4</v>
-      </c>
-      <c r="G10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -616,14 +550,8 @@
       <c r="E11">
         <v>0</v>
       </c>
-      <c r="F11">
-        <v>0</v>
-      </c>
-      <c r="G11">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -639,14 +567,8 @@
       <c r="E12">
         <v>0</v>
       </c>
-      <c r="F12">
-        <v>0</v>
-      </c>
-      <c r="G12">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -662,14 +584,8 @@
       <c r="E13">
         <v>0</v>
       </c>
-      <c r="F13">
-        <v>0</v>
-      </c>
-      <c r="G13">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -677,22 +593,16 @@
         <v>0</v>
       </c>
       <c r="C14">
+        <v>0</v>
+      </c>
+      <c r="D14">
+        <v>2</v>
+      </c>
+      <c r="E14">
         <v>1</v>
       </c>
-      <c r="D14">
-        <v>0</v>
-      </c>
-      <c r="E14">
-        <v>0</v>
-      </c>
-      <c r="F14">
-        <v>2</v>
-      </c>
-      <c r="G14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -700,22 +610,16 @@
         <v>0</v>
       </c>
       <c r="C15">
+        <v>0</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15">
         <v>3</v>
       </c>
-      <c r="D15">
-        <v>0</v>
-      </c>
-      <c r="E15">
-        <v>0</v>
-      </c>
-      <c r="F15">
-        <v>0</v>
-      </c>
-      <c r="G15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -723,22 +627,16 @@
         <v>0</v>
       </c>
       <c r="C16">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D16">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E16">
-        <v>1</v>
-      </c>
-      <c r="F16">
-        <v>3</v>
-      </c>
-      <c r="G16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -746,22 +644,16 @@
         <v>0</v>
       </c>
       <c r="C17">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="D17">
         <v>0</v>
       </c>
       <c r="E17">
-        <v>1</v>
-      </c>
-      <c r="F17">
-        <v>0</v>
-      </c>
-      <c r="G17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2018</v>
       </c>
@@ -769,18 +661,12 @@
         <v>10</v>
       </c>
       <c r="C18">
-        <v>0</v>
+        <v>18</v>
       </c>
       <c r="D18">
         <v>0</v>
       </c>
       <c r="E18">
-        <v>18</v>
-      </c>
-      <c r="F18">
-        <v>0</v>
-      </c>
-      <c r="G18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Enabled fit lmm with CV and comparison plots
</commit_message>
<xml_diff>
--- a/dat/cases/hk_annual_cases_areas.xlsx
+++ b/dat/cases/hk_annual_cases_areas.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\workspace\dengue-forecast-hk\dat\cases\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ksucipto\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,21 +24,24 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>year</t>
-  </si>
-  <si>
-    <t>HK</t>
   </si>
   <si>
     <t>NTS</t>
   </si>
   <si>
+    <t>NTN</t>
+  </si>
+  <si>
+    <t>HKL</t>
+  </si>
+  <si>
     <t>KL</t>
   </si>
   <si>
-    <t>NTN</t>
+    <t>HK</t>
   </si>
 </sst>
 </file>
@@ -356,32 +359,35 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E18"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="E1" sqref="E1:F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="C1" t="s">
         <v>3</v>
       </c>
       <c r="D1" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="E1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>2002</v>
       </c>
@@ -392,13 +398,16 @@
         <v>0</v>
       </c>
       <c r="D2">
-        <v>0</v>
+        <v>20</v>
       </c>
       <c r="E2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2003</v>
       </c>
@@ -409,13 +418,16 @@
         <v>0</v>
       </c>
       <c r="D3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="E3">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2004</v>
       </c>
@@ -431,8 +443,11 @@
       <c r="E4">
         <v>0</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2005</v>
       </c>
@@ -448,8 +463,11 @@
       <c r="E5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>2006</v>
       </c>
@@ -465,8 +483,11 @@
       <c r="E6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>2007</v>
       </c>
@@ -482,8 +503,11 @@
       <c r="E7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>2008</v>
       </c>
@@ -499,8 +523,11 @@
       <c r="E8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2009</v>
       </c>
@@ -516,8 +543,11 @@
       <c r="E9">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F9">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2010</v>
       </c>
@@ -525,16 +555,19 @@
         <v>0</v>
       </c>
       <c r="C10">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10">
+        <v>0</v>
+      </c>
+      <c r="F10">
         <v>4</v>
       </c>
-      <c r="E10">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2011</v>
       </c>
@@ -550,8 +583,11 @@
       <c r="E11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F11">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>2012</v>
       </c>
@@ -567,8 +603,11 @@
       <c r="E12">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F12">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>2013</v>
       </c>
@@ -584,8 +623,11 @@
       <c r="E13">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F13">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>2014</v>
       </c>
@@ -593,16 +635,19 @@
         <v>0</v>
       </c>
       <c r="C14">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D14">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>0</v>
+      </c>
+      <c r="F14">
         <v>2</v>
       </c>
-      <c r="E14">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>2015</v>
       </c>
@@ -613,13 +658,16 @@
         <v>0</v>
       </c>
       <c r="D15">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="E15">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F15">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>2016</v>
       </c>
@@ -627,16 +675,19 @@
         <v>0</v>
       </c>
       <c r="C16">
+        <v>4</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16">
         <v>1</v>
       </c>
-      <c r="D16">
+      <c r="F16">
         <v>3</v>
       </c>
-      <c r="E16">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>2017</v>
       </c>
@@ -650,10 +701,13 @@
         <v>0</v>
       </c>
       <c r="E17">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="F17">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>2018</v>
       </c>
@@ -667,6 +721,9 @@
         <v>0</v>
       </c>
       <c r="E18">
+        <v>18</v>
+      </c>
+      <c r="F18">
         <v>0</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Updated lasso, added CI calculations for paper
</commit_message>
<xml_diff>
--- a/dat/cases/hk_annual_cases_areas.xlsx
+++ b/dat/cases/hk_annual_cases_areas.xlsx
@@ -362,7 +362,7 @@
   <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -392,16 +392,16 @@
         <v>2002</v>
       </c>
       <c r="B2">
+        <v>5</v>
+      </c>
+      <c r="C2">
+        <v>6</v>
+      </c>
+      <c r="D2">
         <v>8</v>
       </c>
-      <c r="C2">
-        <v>0</v>
-      </c>
-      <c r="D2">
-        <v>11</v>
-      </c>
       <c r="E2">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F2">
         <v>0</v>
@@ -715,13 +715,13 @@
         <v>10</v>
       </c>
       <c r="C18">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="E18">
         <v>16</v>
-      </c>
-      <c r="D18">
-        <v>3</v>
-      </c>
-      <c r="E18">
-        <v>18</v>
       </c>
       <c r="F18">
         <v>0</v>

</xml_diff>